<commit_message>
changes in multiple file
</commit_message>
<xml_diff>
--- a/experiment/analysis_31.xlsx
+++ b/experiment/analysis_31.xlsx
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B74"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -400,58 +400,58 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>0.9603013619240799</v>
+        <v>0.9255213505461769</v>
       </c>
       <c r="B2">
-        <v>1685534987.032359</v>
+        <v>1685613059.095365</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>0.9687047232686177</v>
+        <v>0.006620324395895399</v>
       </c>
       <c r="B3">
-        <v>1685534988.039695</v>
+        <v>1685613060.103559</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>0.9603013619240799</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>1685534989.04455</v>
+        <v>1685613061.113617</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>0.0651984931903796</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>1685534990.05957</v>
+        <v>1685613062.11815</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.05940307157345697</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>1685534991.068129</v>
+        <v>1685613063.124629</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.05679513184584178</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>1685534992.076792</v>
+        <v>1685613064.130596</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>0</v>
+        <v>0.9804700430321087</v>
       </c>
       <c r="B8">
-        <v>1685534993.07779</v>
+        <v>1685613065.136958</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -459,7 +459,7 @@
         <v>0</v>
       </c>
       <c r="B9">
-        <v>1685534994.086077</v>
+        <v>1685613066.137494</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -467,7 +467,7 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>1685534995.098873</v>
+        <v>1685613067.141251</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -475,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <v>1685534996.103348</v>
+        <v>1685613068.145785</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -483,15 +483,15 @@
         <v>0</v>
       </c>
       <c r="B12">
-        <v>1685534997.110153</v>
+        <v>1685613069.149947</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>1</v>
+        <v>0.9837802052300564</v>
       </c>
       <c r="B13">
-        <v>1685534998.120677</v>
+        <v>1685613070.157634</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -499,7 +499,7 @@
         <v>0</v>
       </c>
       <c r="B14">
-        <v>1685534999.133454</v>
+        <v>1685613071.159661</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -507,7 +507,7 @@
         <v>0</v>
       </c>
       <c r="B15">
-        <v>1685535000.139917</v>
+        <v>1685613072.168591</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -515,23 +515,23 @@
         <v>0</v>
       </c>
       <c r="B16">
-        <v>1685535001.151649</v>
+        <v>1685613073.177304</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>0.1501014198782961</v>
+        <v>0.3978814961933135</v>
       </c>
       <c r="B17">
-        <v>1685535002.158641</v>
+        <v>1685613074.178235</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>0.4957983193277311</v>
+        <v>0.6858656074147633</v>
       </c>
       <c r="B18">
-        <v>1685535003.164979</v>
+        <v>1685613075.180999</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="B19">
-        <v>1685535004.177079</v>
+        <v>1685613076.185697</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -547,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="B20">
-        <v>1685535005.187091</v>
+        <v>1685613077.193296</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -555,23 +555,23 @@
         <v>0</v>
       </c>
       <c r="B21">
-        <v>1685535006.192605</v>
+        <v>1685613078.200558</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>0.7166038829324832</v>
+        <v>0.5954981794107912</v>
       </c>
       <c r="B22">
-        <v>1685535007.198736</v>
+        <v>1685613079.207412</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>0.1445957693422196</v>
+        <v>0.1780867262495862</v>
       </c>
       <c r="B23">
-        <v>1685535008.206399</v>
+        <v>1685613080.211111</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -579,7 +579,7 @@
         <v>0</v>
       </c>
       <c r="B24">
-        <v>1685535009.213585</v>
+        <v>1685613081.225981</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -587,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="B25">
-        <v>1685535010.222224</v>
+        <v>1685613082.240733</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -595,23 +595,23 @@
         <v>0</v>
       </c>
       <c r="B26">
-        <v>1685535011.231252</v>
+        <v>1685613083.247193</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>0.8498985801217038</v>
+        <v>0.7861635220125787</v>
       </c>
       <c r="B27">
-        <v>1685535012.231776</v>
+        <v>1685613084.253564</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>0.07360185453491741</v>
+        <v>0.08738828202581927</v>
       </c>
       <c r="B28">
-        <v>1685535013.240928</v>
+        <v>1685613085.255706</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="B29">
-        <v>1685535014.243321</v>
+        <v>1685613086.259642</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -627,7 +627,7 @@
         <v>0</v>
       </c>
       <c r="B30">
-        <v>1685535015.250641</v>
+        <v>1685613087.267441</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -635,23 +635,23 @@
         <v>0</v>
       </c>
       <c r="B31">
-        <v>1685535016.259624</v>
+        <v>1685613088.271025</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>0.8753984352361633</v>
+        <v>0.8639523336643496</v>
       </c>
       <c r="B32">
-        <v>1685535017.266661</v>
+        <v>1685613089.279618</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>0.03680092726745871</v>
+        <v>0.04203905991393578</v>
       </c>
       <c r="B33">
-        <v>1685535018.27216</v>
+        <v>1685613090.284304</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -659,7 +659,7 @@
         <v>0</v>
       </c>
       <c r="B34">
-        <v>1685535019.279896</v>
+        <v>1685613091.293627</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="B35">
-        <v>1685535020.28748</v>
+        <v>1685613092.300772</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -675,23 +675,23 @@
         <v>0</v>
       </c>
       <c r="B36">
-        <v>1685535021.294036</v>
+        <v>1685613093.304582</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>0.9093016516951609</v>
+        <v>0.9155908639523338</v>
       </c>
       <c r="B37">
-        <v>1685535022.301654</v>
+        <v>1685613094.310327</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>0.03390321645899739</v>
+        <v>0.03872889771598809</v>
       </c>
       <c r="B38">
-        <v>1685535023.306973</v>
+        <v>1685613095.326353</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -699,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="B39">
-        <v>1685535024.313986</v>
+        <v>1685613096.333715</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="B40">
-        <v>1685535025.323688</v>
+        <v>1685613097.343356</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -715,23 +715,23 @@
         <v>0</v>
       </c>
       <c r="B41">
-        <v>1685535026.337599</v>
+        <v>1685613098.354654</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>0.931903796001159</v>
+        <v>0.9318106587222774</v>
       </c>
       <c r="B42">
-        <v>1685535027.346315</v>
+        <v>1685613099.361206</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>0.02260214430599826</v>
+        <v>0.02581926514399206</v>
       </c>
       <c r="B43">
-        <v>1685535028.354643</v>
+        <v>1685613100.364231</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="B44">
-        <v>1685535029.363429</v>
+        <v>1685613101.368996</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -747,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="B45">
-        <v>1685535030.37066</v>
+        <v>1685613102.377042</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -755,23 +755,23 @@
         <v>0</v>
       </c>
       <c r="B46">
-        <v>1685535031.378352</v>
+        <v>1685613103.378177</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>0.9376992176180816</v>
+        <v>0.9351208209202251</v>
       </c>
       <c r="B47">
-        <v>1685535032.386641</v>
+        <v>1685613104.384887</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>0.01419878296146044</v>
+        <v>0.02250910294604436</v>
       </c>
       <c r="B48">
-        <v>1685535033.392559</v>
+        <v>1685613105.389002</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="B49">
-        <v>1685535034.39964</v>
+        <v>1685613106.394259</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -787,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="B50">
-        <v>1685535035.409538</v>
+        <v>1685613107.395642</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -795,23 +795,23 @@
         <v>0</v>
       </c>
       <c r="B51">
-        <v>1685535036.418397</v>
+        <v>1685613108.398235</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>0.9461025789626195</v>
+        <v>0.9384309831181727</v>
       </c>
       <c r="B52">
-        <v>1685535037.430641</v>
+        <v>1685613109.403816</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
-        <v>0.01130107215299913</v>
+        <v>0.01621979476994373</v>
       </c>
       <c r="B53">
-        <v>1685535038.438529</v>
+        <v>1685613110.417581</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="B54">
-        <v>1685535039.450719</v>
+        <v>1685613111.423888</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -827,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="B55">
-        <v>1685535040.463537</v>
+        <v>1685613112.431649</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -835,23 +835,23 @@
         <v>0</v>
       </c>
       <c r="B56">
-        <v>1685535041.470818</v>
+        <v>1685613113.435671</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <v>0.9545059403071574</v>
+        <v>0.9513406156901688</v>
       </c>
       <c r="B57">
-        <v>1685535042.482666</v>
+        <v>1685613114.444269</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <v>0.008403361344537815</v>
+        <v>0.01290963257199603</v>
       </c>
       <c r="B58">
-        <v>1685535043.492624</v>
+        <v>1685613115.449906</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="B59">
-        <v>1685535044.501785</v>
+        <v>1685613116.450998</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -867,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="B60">
-        <v>1685535045.50901</v>
+        <v>1685613117.451643</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -875,111 +875,71 @@
         <v>0</v>
       </c>
       <c r="B61">
-        <v>1685535046.521168</v>
+        <v>1685613118.454959</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>0.9545059403071574</v>
+        <v>0.9609400860642172</v>
       </c>
       <c r="B62">
-        <v>1685535047.529928</v>
+        <v>1685613119.456368</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>0.002897710808461316</v>
+        <v>0.9966898378020523</v>
       </c>
       <c r="B63">
-        <v>1685535048.53676</v>
+        <v>1685613120.471049</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>0</v>
+        <v>0.9966898378020523</v>
       </c>
       <c r="B64">
-        <v>1685535049.547781</v>
+        <v>1685613121.474754</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>0</v>
+        <v>0.9867593512082092</v>
       </c>
       <c r="B65">
-        <v>1685535050.55584</v>
+        <v>1685613122.482967</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B66">
-        <v>1685535051.563881</v>
+        <v>1685613123.491504</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>0.9574036511156186</v>
+        <v>0.9966898378020523</v>
       </c>
       <c r="B67">
-        <v>1685535052.572542</v>
+        <v>1685613124.500623</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>0.9603013619240799</v>
+        <v>0.9966898378020523</v>
       </c>
       <c r="B68">
-        <v>1685535053.578573</v>
+        <v>1685613125.506711</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>0.9745001448855404</v>
+        <v>0.9966898378020523</v>
       </c>
       <c r="B69">
-        <v>1685535054.582942</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70">
-        <v>0.9687047232686177</v>
-      </c>
-      <c r="B70">
-        <v>1685535055.588851</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71">
-        <v>0.971602434077079</v>
-      </c>
-      <c r="B71">
-        <v>1685535056.601307</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72">
-        <v>0.9687047232686177</v>
-      </c>
-      <c r="B72">
-        <v>1685535057.610351</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73">
-        <v>0.9658070124601564</v>
-      </c>
-      <c r="B73">
-        <v>1685535058.620931</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74">
-        <v>0.9687047232686177</v>
-      </c>
-      <c r="B74">
-        <v>1685535059.633821</v>
+        <v>1685613126.521278</v>
       </c>
     </row>
   </sheetData>
@@ -989,7 +949,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1005,658 +965,282 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>0.129265086239452</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>1685515925.231202</v>
+        <v>1685613065.147663</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>0.1273822873449297</v>
+        <v>0.2576240895316762</v>
       </c>
       <c r="B3">
-        <v>1685515926.325259</v>
+        <v>1685613066.168225</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>0.1277591894560915</v>
+        <v>0.9990026438706784</v>
       </c>
       <c r="B4">
-        <v>1685515927.433166</v>
+        <v>1685613070.226218</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>0.1264853412592519</v>
+        <v>0.2366326840975001</v>
       </c>
       <c r="B5">
-        <v>1685515928.527225</v>
+        <v>1685613071.236143</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.1266312532521254</v>
+        <v>0.9685660658364204</v>
       </c>
       <c r="B6">
-        <v>1685515929.623169</v>
+        <v>1685613075.286364</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.1276582185320411</v>
+        <v>0.2282862857085139</v>
       </c>
       <c r="B7">
-        <v>1685515930.716222</v>
+        <v>1685613076.295844</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>0.1263484786221036</v>
+        <v>0.2215038182014743</v>
       </c>
       <c r="B8">
-        <v>1685515931.81023</v>
+        <v>1685613078.340245</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>0.1287373268262374</v>
+        <v>0.2099154640889067</v>
       </c>
       <c r="B9">
-        <v>1685515932.90422</v>
+        <v>1685613079.350001</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>0.1460273744357581</v>
+        <v>0.8449838342062587</v>
       </c>
       <c r="B10">
-        <v>1685515933.998177</v>
+        <v>1685613080.360299</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>1</v>
+        <v>0.2281233416472198</v>
       </c>
       <c r="B11">
-        <v>1685515935.093256</v>
+        <v>1685613081.360224</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>0.2626610633331705</v>
+        <v>0.3218212871724346</v>
       </c>
       <c r="B12">
-        <v>1685515936.185952</v>
+        <v>1685613084.40032</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>0.1496251859113984</v>
+        <v>0.7789696718830714</v>
       </c>
       <c r="B13">
-        <v>1685515937.2786</v>
+        <v>1685613085.410274</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>0.1331930081069563</v>
+        <v>0.2180567303606938</v>
       </c>
       <c r="B14">
-        <v>1685515938.372293</v>
+        <v>1685613086.420332</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>0.5691455831765331</v>
+        <v>0.4153476349830282</v>
       </c>
       <c r="B15">
-        <v>1685515939.473251</v>
+        <v>1685613089.45035</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>0.4926625569570685</v>
+        <v>0.7162498568579189</v>
       </c>
       <c r="B16">
-        <v>1685515940.56619</v>
+        <v>1685613090.46981</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>0.1863267630315393</v>
+        <v>0.2130035600387493</v>
       </c>
       <c r="B17">
-        <v>1685515941.659991</v>
+        <v>1685613091.480011</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>0.1395133682347507</v>
+        <v>0.480450475922496</v>
       </c>
       <c r="B18">
-        <v>1685515942.794955</v>
+        <v>1685613094.510285</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>0.1338628247055755</v>
+        <v>0.661700684247443</v>
       </c>
       <c r="B19">
-        <v>1685515943.889198</v>
+        <v>1685613095.519966</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>0.9343390253820049</v>
+        <v>0.2122461348749667</v>
       </c>
       <c r="B20">
-        <v>1685515944.981794</v>
+        <v>1685613096.530032</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>0.2718846638080766</v>
+        <v>0.5741955863475671</v>
       </c>
       <c r="B21">
-        <v>1685515946.076133</v>
+        <v>1685613099.569975</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>0.1567467671975583</v>
+        <v>0.6053373621984545</v>
       </c>
       <c r="B22">
-        <v>1685515947.209759</v>
+        <v>1685613100.580904</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>0.1391434068239473</v>
+        <v>0.198198589246505</v>
       </c>
       <c r="B23">
-        <v>1685515948.335956</v>
+        <v>1685613101.590235</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>0.5370761976154419</v>
+        <v>0.6310611874371139</v>
       </c>
       <c r="B24">
-        <v>1685515949.445307</v>
+        <v>1685613104.620124</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>0.5059549311588837</v>
+        <v>0.5631138768644532</v>
       </c>
       <c r="B25">
-        <v>1685515950.544163</v>
+        <v>1685613105.640294</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>0.1932975440179551</v>
+        <v>0.1932092874543898</v>
       </c>
       <c r="B26">
-        <v>1685515951.654186</v>
+        <v>1685613106.650166</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>0.1462148498925832</v>
+        <v>0.7073607163076321</v>
       </c>
       <c r="B27">
-        <v>1685515952.747199</v>
+        <v>1685613109.679727</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>0.1432611674868057</v>
+        <v>0.5212184377595389</v>
       </c>
       <c r="B28">
-        <v>1685515953.841212</v>
+        <v>1685613110.689708</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>0.9458963218143238</v>
+        <v>0.1858963806701341</v>
       </c>
       <c r="B29">
-        <v>1685515954.934191</v>
+        <v>1685613111.700327</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>0.2903708651238266</v>
+        <v>0.7641226159436726</v>
       </c>
       <c r="B30">
-        <v>1685515956.028693</v>
+        <v>1685613114.760316</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>0.1634675202233731</v>
+        <v>0.4992895078097414</v>
       </c>
       <c r="B31">
-        <v>1685515957.125179</v>
+        <v>1685613115.770596</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>0.145047809879707</v>
+        <v>0.1876875999807831</v>
       </c>
       <c r="B32">
-        <v>1685515958.217893</v>
+        <v>1685613116.780206</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>0.3730964159684522</v>
+        <v>0.2272963635397318</v>
       </c>
       <c r="B33">
-        <v>1685515959.312168</v>
+        <v>1685613117.790304</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>0.6098245550050667</v>
+        <v>0.8028524501304349</v>
       </c>
       <c r="B34">
-        <v>1685515960.405734</v>
+        <v>1685613119.810278</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>0.225325125019827</v>
+        <v>0.4238941070398836</v>
       </c>
       <c r="B35">
-        <v>1685515961.502183</v>
+        <v>1685613120.820335</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>0.1592895126435416</v>
+        <v>0.1792086538909354</v>
       </c>
       <c r="B36">
-        <v>1685515962.595923</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37">
-        <v>0.1480212903981764</v>
-      </c>
-      <c r="B37">
-        <v>1685515963.693271</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38">
-        <v>0.8254427455465677</v>
-      </c>
-      <c r="B38">
-        <v>1685515964.787098</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39">
-        <v>0.3350772677334053</v>
-      </c>
-      <c r="B39">
-        <v>1685515965.88023</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40">
-        <v>0.1759458250816958</v>
-      </c>
-      <c r="B40">
-        <v>1685515967.152688</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41">
-        <v>0.1519863082129666</v>
-      </c>
-      <c r="B41">
-        <v>1685515968.278678</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42">
-        <v>0.4917431500357904</v>
-      </c>
-      <c r="B42">
-        <v>1685515969.410275</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43">
-        <v>0.51651976954537</v>
-      </c>
-      <c r="B43">
-        <v>1685515970.525265</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44">
-        <v>0.2036960261130679</v>
-      </c>
-      <c r="B44">
-        <v>1685515971.646193</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45">
-        <v>0.1571075393045497</v>
-      </c>
-      <c r="B45">
-        <v>1685515972.756241</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46">
-        <v>0.1489683625408121</v>
-      </c>
-      <c r="B46">
-        <v>1685515973.849926</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47">
-        <v>0.9203026583510776</v>
-      </c>
-      <c r="B47">
-        <v>1685515974.943456</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48">
-        <v>0.2821398075820352</v>
-      </c>
-      <c r="B48">
-        <v>1685515976.063178</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49">
-        <v>0.1684587449467872</v>
-      </c>
-      <c r="B49">
-        <v>1685515977.158195</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50">
-        <v>0.1510650955027933</v>
-      </c>
-      <c r="B50">
-        <v>1685515978.251354</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51">
-        <v>0.4185486625939026</v>
-      </c>
-      <c r="B51">
-        <v>1685515979.345191</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52">
-        <v>0.5855746612542632</v>
-      </c>
-      <c r="B52">
-        <v>1685515980.438188</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53">
-        <v>0.2132038499164612</v>
-      </c>
-      <c r="B53">
-        <v>1685515981.53318</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54">
-        <v>0.1578815961721895</v>
-      </c>
-      <c r="B54">
-        <v>1685515982.626897</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55">
-        <v>0.1497081615278138</v>
-      </c>
-      <c r="B55">
-        <v>1685515983.720949</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56">
-        <v>0.8563841892920089</v>
-      </c>
-      <c r="B56">
-        <v>1685515984.829245</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57">
-        <v>0.3215623640936274</v>
-      </c>
-      <c r="B57">
-        <v>1685515985.923224</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58">
-        <v>0.1745108830653265</v>
-      </c>
-      <c r="B58">
-        <v>1685515987.01739</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59">
-        <v>0.1512566618640598</v>
-      </c>
-      <c r="B59">
-        <v>1685515988.110284</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60">
-        <v>0.20728658470672</v>
-      </c>
-      <c r="B60">
-        <v>1685515989.206279</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61">
-        <v>0.704263790300418</v>
-      </c>
-      <c r="B61">
-        <v>1685515990.300225</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62">
-        <v>0.229921563253127</v>
-      </c>
-      <c r="B62">
-        <v>1685515991.393403</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63">
-        <v>0.1569581241309086</v>
-      </c>
-      <c r="B63">
-        <v>1685515992.486352</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64">
-        <v>0.1489109890451841</v>
-      </c>
-      <c r="B64">
-        <v>1685515993.579522</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65">
-        <v>0.1464915519884942</v>
-      </c>
-      <c r="B65">
-        <v>1685515994.675544</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66">
-        <v>0.1459755456381152</v>
-      </c>
-      <c r="B66">
-        <v>1685515995.76945</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67">
-        <v>0.1455439893838858</v>
-      </c>
-      <c r="B67">
-        <v>1685515996.865471</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68">
-        <v>0.144953729837516</v>
-      </c>
-      <c r="B68">
-        <v>1685515997.960932</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69">
-        <v>0.1437546807703575</v>
-      </c>
-      <c r="B69">
-        <v>1685515999.055261</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70">
-        <v>0.143061075764928</v>
-      </c>
-      <c r="B70">
-        <v>1685516000.149109</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71">
-        <v>0.1428424219948866</v>
-      </c>
-      <c r="B71">
-        <v>1685516001.243978</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72">
-        <v>0.1420108065433727</v>
-      </c>
-      <c r="B72">
-        <v>1685516002.337529</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73">
-        <v>0.1416652086220715</v>
-      </c>
-      <c r="B73">
-        <v>1685516003.431234</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74">
-        <v>0.1437079885099412</v>
-      </c>
-      <c r="B74">
-        <v>1685516004.524847</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75">
-        <v>0.2379300688266499</v>
-      </c>
-      <c r="B75">
-        <v>1685516005.619005</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76">
-        <v>0.1392058204481784</v>
-      </c>
-      <c r="B76">
-        <v>1685516006.714171</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77">
-        <v>0.1242787579147139</v>
-      </c>
-      <c r="B77">
-        <v>1685516007.80629</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78">
-        <v>0.1214338945905142</v>
-      </c>
-      <c r="B78">
-        <v>1685516008.899967</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79">
-        <v>0.1236363609657477</v>
-      </c>
-      <c r="B79">
-        <v>1685516009.992843</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80">
-        <v>0.1195240150526035</v>
-      </c>
-      <c r="B80">
-        <v>1685516011.087283</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81">
-        <v>0.1182321069846134</v>
-      </c>
-      <c r="B81">
-        <v>1685516012.180349</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82">
-        <v>0.117701770721372</v>
-      </c>
-      <c r="B82">
-        <v>1685516013.27523</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83">
-        <v>0.1011876829076786</v>
-      </c>
-      <c r="B83">
-        <v>1685516014.369259</v>
+        <v>1685613121.839892</v>
       </c>
     </row>
   </sheetData>

</xml_diff>